<commit_message>
Test Case - Spring 5
Correct version of the test case to the spring 5
</commit_message>
<xml_diff>
--- a/test-case.xlsx
+++ b/test-case.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="51">
   <si>
     <t>TC1</t>
   </si>
@@ -129,12 +129,12 @@
     <t>Tested By</t>
   </si>
   <si>
-    <t>Patient-Clinical Data</t>
-  </si>
-  <si>
     <t>Irvin</t>
   </si>
   <si>
+    <t>To be able to view detailed information of the restaurant clicked</t>
+  </si>
+  <si>
     <t>Efficient position and styling for pictures in detail screens</t>
   </si>
   <si>
@@ -156,6 +156,12 @@
     <t>Expected appearance of pictures on the two screens along with the photo section in details.</t>
   </si>
   <si>
+    <t>Implement backend yelp API call to retrieve pictures information</t>
+  </si>
+  <si>
+    <t>Appropriate pictures of each restaurant are displayed in detail.</t>
+  </si>
+  <si>
     <t>Call detail screen when you tap on the popup of map screen</t>
   </si>
   <si>
@@ -165,19 +171,34 @@
     <t>On clicking on map, popup appears, on further clicking on popup it shoulfd open the detail screen of the restaurant clicked.</t>
   </si>
   <si>
-    <t>Restaurant's price category will be shown in List and Details screen.</t>
+    <t>TC5</t>
+  </si>
+  <si>
+    <t>Sergio Brunacci</t>
   </si>
   <si>
     <t>Appetite</t>
   </si>
   <si>
-    <t>To be able to view price category for a choose restaurant in the list and detail screens.</t>
-  </si>
-  <si>
-    <t>Open the list of restaurants and their details and check the information about price category.</t>
-  </si>
-  <si>
-    <t>Sergio Brunacci</t>
+    <t>TC6</t>
+  </si>
+  <si>
+    <t>Restaurant's price category will be shown in the list of restaurants.</t>
+  </si>
+  <si>
+    <t>Open the list of restaurants and check the information about price category.</t>
+  </si>
+  <si>
+    <t>To be able to view price category for a choose restaurant in the list screen.</t>
+  </si>
+  <si>
+    <t>Restaurant's price category will be shown in the Details screen.</t>
+  </si>
+  <si>
+    <t>Open the details screen and check the information about price category.</t>
+  </si>
+  <si>
+    <t>To be able to view price category for a choose restaurant in the detail screen.</t>
   </si>
 </sst>
 </file>
@@ -3548,10 +3569,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -3572,9 +3593,7 @@
       <c r="A2" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="54" t="s">
-        <v>40</v>
-      </c>
+      <c r="B2" s="54"/>
       <c r="C2" s="54"/>
       <c r="D2" s="55"/>
       <c r="E2" s="29"/>
@@ -3589,14 +3608,14 @@
         <v>24</v>
       </c>
       <c r="B3" s="44">
-        <f>COUNTIF(I8:I24,"Pass")</f>
-        <v>4</v>
+        <f>COUNTIF(I8:I12,"Pass")</f>
+        <v>5</v>
       </c>
       <c r="C3" s="44" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="45">
-        <f>COUNTIF(I7:I682,"Pending")</f>
+        <f>COUNTIF(I7:I669,"Pending")</f>
         <v>0</v>
       </c>
       <c r="E3" s="3"/>
@@ -3618,8 +3637,8 @@
         <v>19</v>
       </c>
       <c r="D4" s="48">
-        <f>COUNTA(A8:A24)</f>
-        <v>4</v>
+        <f>COUNTA(A8:A12)</f>
+        <v>5</v>
       </c>
       <c r="E4" s="30"/>
       <c r="F4" s="30"/>
@@ -3696,7 +3715,7 @@
       <c r="E8" s="52"/>
       <c r="F8" s="53"/>
       <c r="G8" s="38" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H8" s="50" t="s">
         <v>33</v>
@@ -3722,7 +3741,7 @@
       <c r="E9" s="52"/>
       <c r="F9" s="53"/>
       <c r="G9" s="38" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H9" s="50" t="s">
         <v>33</v>
@@ -3737,18 +3756,18 @@
         <v>2</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C10" s="38" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D10" s="51" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E10" s="52"/>
       <c r="F10" s="53"/>
       <c r="G10" s="38" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="H10" s="50" t="s">
         <v>34</v>
@@ -3763,18 +3782,18 @@
         <v>3</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C11" s="38" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D11" s="51" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E11" s="52"/>
       <c r="F11" s="53"/>
       <c r="G11" s="38" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H11" s="50" t="s">
         <v>33</v>
@@ -3784,172 +3803,66 @@
       </c>
       <c r="J11" s="38"/>
     </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="38"/>
-      <c r="B12" s="38"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="51"/>
+    <row r="12" spans="1:10" ht="43" customHeight="1">
+      <c r="A12" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="51" t="s">
+        <v>47</v>
+      </c>
       <c r="E12" s="52"/>
       <c r="F12" s="53"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="50"/>
-      <c r="I12" s="38"/>
+      <c r="G12" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="H12" s="50" t="s">
+        <v>33</v>
+      </c>
+      <c r="I12" s="38" t="s">
+        <v>24</v>
+      </c>
       <c r="J12" s="38"/>
     </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="38"/>
-      <c r="B13" s="38"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="51"/>
+    <row r="13" spans="1:10" ht="43" customHeight="1">
+      <c r="A13" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="51" t="s">
+        <v>50</v>
+      </c>
       <c r="E13" s="52"/>
       <c r="F13" s="53"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="50"/>
-      <c r="I13" s="38"/>
+      <c r="G13" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13" s="50" t="s">
+        <v>33</v>
+      </c>
+      <c r="I13" s="38" t="s">
+        <v>24</v>
+      </c>
       <c r="J13" s="38"/>
     </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="38"/>
-      <c r="B14" s="38"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="52"/>
-      <c r="F14" s="53"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="50"/>
-      <c r="I14" s="38"/>
-      <c r="J14" s="38"/>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="38"/>
-      <c r="B15" s="38"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="53"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="50"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="38"/>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="38"/>
-      <c r="B16" s="38"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="51"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="53"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="50"/>
-      <c r="I16" s="38"/>
-      <c r="J16" s="38"/>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="38"/>
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="51"/>
-      <c r="E17" s="52"/>
-      <c r="F17" s="53"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="50"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="38"/>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="38"/>
-      <c r="B18" s="38"/>
-      <c r="C18" s="38"/>
-      <c r="D18" s="51"/>
-      <c r="E18" s="52"/>
-      <c r="F18" s="53"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="50"/>
-      <c r="I18" s="38"/>
-      <c r="J18" s="38"/>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="38"/>
-      <c r="B19" s="38"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="51"/>
-      <c r="E19" s="52"/>
-      <c r="F19" s="53"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="50"/>
-      <c r="I19" s="38"/>
-      <c r="J19" s="38"/>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="38"/>
-      <c r="B20" s="38"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="52"/>
-      <c r="F20" s="53"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="50"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="38"/>
-      <c r="B21" s="38"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="51"/>
-      <c r="E21" s="52"/>
-      <c r="F21" s="53"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="50"/>
-      <c r="I21" s="38"/>
-      <c r="J21" s="38"/>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="38"/>
-      <c r="B22" s="38"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="51"/>
-      <c r="E22" s="52"/>
-      <c r="F22" s="53"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="50"/>
-      <c r="I22" s="38"/>
-      <c r="J22" s="38"/>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="38"/>
-      <c r="B23" s="38"/>
-      <c r="C23" s="38"/>
-      <c r="D23" s="51"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="53"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="50"/>
-      <c r="I23" s="38"/>
-      <c r="J23" s="38"/>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="38"/>
-      <c r="B24" s="38"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="51"/>
-      <c r="E24" s="52"/>
-      <c r="F24" s="53"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="50"/>
-      <c r="I24" s="38"/>
-      <c r="J24" s="38"/>
-    </row>
   </sheetData>
-  <mergeCells count="30">
-    <mergeCell ref="D15:F15"/>
+  <mergeCells count="19">
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D9:F9"/>
     <mergeCell ref="D8:F8"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="D6:F7"/>
-    <mergeCell ref="D17:F17"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="H2:J2"/>
@@ -3961,17 +3874,8 @@
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="D12:F12"/>
     <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D14:F14"/>
     <mergeCell ref="D10:F10"/>
-    <mergeCell ref="D16:F16"/>
     <mergeCell ref="A6:A7"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D22:F22"/>
   </mergeCells>
   <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3985,7 +3889,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -4079,11 +3983,11 @@
         <v>1</v>
       </c>
       <c r="C8" s="34" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="D8" s="35">
         <f>'Sprint-5'!B3</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E8" s="34">
         <f>'Sprint-5'!B4</f>
@@ -4095,7 +3999,7 @@
       </c>
       <c r="G8" s="35">
         <f>'Sprint-5'!D4</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -4115,7 +4019,7 @@
       </c>
       <c r="D10" s="25">
         <f>SUM(D6:D9)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E10" s="25">
         <f>SUM(E6:E9)</f>
@@ -4127,7 +4031,7 @@
       </c>
       <c r="G10" s="26">
         <f>SUM(G6:G9)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:7">

</xml_diff>